<commit_message>
car search test case
checked for additional search parameters
removed unused namespaces from files
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Description</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Search</t>
   </si>
   <si>
-    <t>Booking of car for CURRENT LOCATION with same pickup and drop on airport with additional option of rental company.</t>
-  </si>
-  <si>
     <t>PickUpType-Location</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Airport-LAS</t>
   </si>
   <si>
-    <t>Airport-LAX</t>
-  </si>
-  <si>
     <t>10|20</t>
   </si>
   <si>
@@ -88,10 +82,22 @@
     <t>DestinationLocation</t>
   </si>
   <si>
-    <t>Las Vegas, NV, US - McCarran International Airport (LAS)</t>
-  </si>
-  <si>
-    <t>Los Angeles, CA - Los Angeles International Airport (LAX)</t>
+    <t>SameAsPickUp</t>
+  </si>
+  <si>
+    <t>City-Las  Vegas, NV, US</t>
+  </si>
+  <si>
+    <t>City-Dfw  Airport, TX, US</t>
+  </si>
+  <si>
+    <t>Booking of car for CURRENT LOCATION with same pickup and drop on airport with all additional options selected</t>
+  </si>
+  <si>
+    <t>Booking of car for CURRENT LOCATION with City as pickup and drop on airport with all additional options selected</t>
+  </si>
+  <si>
+    <t>Booking of car for CURRENT LOCATION with Airport as pickup and drop in City with all additional options selected</t>
   </si>
 </sst>
 </file>
@@ -113,12 +119,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -185,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -200,14 +212,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -215,6 +232,94 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -232,6 +337,79 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -246,163 +424,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -522,23 +543,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:N2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="A1:N2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:N4" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:N4"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="Description" dataDxfId="3"/>
+    <tableColumn id="1" name="Description" dataDxfId="0"/>
     <tableColumn id="16" name="ExecutionPipeline" dataDxfId="13"/>
     <tableColumn id="2" name="PickUpType-Location" dataDxfId="12"/>
-    <tableColumn id="19" name="OriginLocation" dataDxfId="1"/>
-    <tableColumn id="3" name="DropOffType-Location" dataDxfId="11"/>
-    <tableColumn id="20" name="DestinationLocation" dataDxfId="0"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="10"/>
-    <tableColumn id="5" name="RentalAgency" dataDxfId="9"/>
-    <tableColumn id="18" name="CarType" dataDxfId="2"/>
-    <tableColumn id="6" name="AirConditioning" dataDxfId="8"/>
-    <tableColumn id="7" name="Transmission" dataDxfId="7"/>
-    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="6"/>
-    <tableColumn id="9" name="CorpDiscCode" dataDxfId="5"/>
-    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="4"/>
+    <tableColumn id="19" name="OriginLocation" dataDxfId="11"/>
+    <tableColumn id="3" name="DropOffType-Location" dataDxfId="10"/>
+    <tableColumn id="20" name="DestinationLocation" dataDxfId="9"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="8"/>
+    <tableColumn id="5" name="RentalAgency" dataDxfId="7"/>
+    <tableColumn id="18" name="CarType" dataDxfId="6"/>
+    <tableColumn id="6" name="AirConditioning" dataDxfId="5"/>
+    <tableColumn id="7" name="Transmission" dataDxfId="4"/>
+    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="3"/>
+    <tableColumn id="9" name="CorpDiscCode" dataDxfId="2"/>
+    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -831,22 +852,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="E15" sqref="E15"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" style="10" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" style="13" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="10" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -858,73 +879,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>23</v>
+      <c r="F1" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>5</v>
+      <c r="A2" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>2</v>
@@ -933,16 +950,96 @@
         <v>1</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parsed car result page
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Description</t>
   </si>
@@ -98,13 +98,31 @@
   </si>
   <si>
     <t>Booking of car for CURRENT LOCATION with Airport as pickup and drop in City with all additional options selected</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>CarSearch_City</t>
+  </si>
+  <si>
+    <t>CarSearch_Airport</t>
+  </si>
+  <si>
+    <t>CarSearch_Airport_SameAsPickUp</t>
+  </si>
+  <si>
+    <t>Las Vegas, NV, US</t>
+  </si>
+  <si>
+    <t>Airport-LAX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +135,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -197,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -226,12 +250,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -482,6 +522,9 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -543,10 +586,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:N4" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="A1:N4"/>
-  <tableColumns count="14">
-    <tableColumn id="1" name="Description" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:O4" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:O4"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Description" dataDxfId="14"/>
+    <tableColumn id="11" name="Type" dataDxfId="0"/>
     <tableColumn id="16" name="ExecutionPipeline" dataDxfId="13"/>
     <tableColumn id="2" name="PickUpType-Location" dataDxfId="12"/>
     <tableColumn id="19" name="OriginLocation" dataDxfId="11"/>
@@ -852,193 +896,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="A3" sqref="A3"/>
+      <selection pane="topRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.5703125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="77.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="14"/>
+      <c r="F3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="4" t="b">
+      <c r="K3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="4" t="b">
+      <c r="K4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix for adult age and added methods to set car filters and matrix
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="881" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="881"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Airport_To_Airport" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Car_City_To_Airport" sheetId="4" r:id="rId4"/>
     <sheet name="Car_City_To_City" sheetId="5" r:id="rId5"/>
     <sheet name="Car_City_To_SameAsPickUp" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -96,16 +97,7 @@
     <t>Guest</t>
   </si>
   <si>
-    <t>Booking of car for pickup on Airport and drop on airport with all additional options selected</t>
-  </si>
-  <si>
-    <t>Booking of car for pickup on Airport and drop in a City with all additional options selected</t>
-  </si>
-  <si>
     <t>City-LAX</t>
-  </si>
-  <si>
-    <t>Booking of car for pickup on Airport and drop SameAsPickUp with all additional options selected</t>
   </si>
   <si>
     <t>Booking of car for pickup in a City and drop on airport with all additional options selected</t>
@@ -129,10 +121,49 @@
     <t>PostFiltersValues</t>
   </si>
   <si>
-    <t>price</t>
+    <t>Avis/Hertz</t>
   </si>
   <si>
-    <t>20-30</t>
+    <t>CarOptions</t>
+  </si>
+  <si>
+    <t>EAC/EAT</t>
+  </si>
+  <si>
+    <t>price|locations|CarType|RentalAgency|CarOptions|matrix</t>
+  </si>
+  <si>
+    <t>SameAsPickup</t>
+  </si>
+  <si>
+    <t>20-30|Off Terminal|Economy/Compact|Avis/Hertz|EAC/EAT</t>
+  </si>
+  <si>
+    <t>Car_WithLoginMember_DOMESTIC_Location_SamePickup_DropAirport</t>
+  </si>
+  <si>
+    <t>Car_WithLoginMember_DOMESTIC_Location_DifferentPickup_DropAirport</t>
+  </si>
+  <si>
+    <t>Registered</t>
+  </si>
+  <si>
+    <t>Car_WithLoginMember_DOMESTIC_Location_SamePickupAndDrop_InACity</t>
+  </si>
+  <si>
+    <t>Car_WithLoginMember_DOMESTIC_Location_DifferentPickupAndDrop_InACity</t>
+  </si>
+  <si>
+    <t>Car_WithGuestUser_DOMESTIC_Location_SamePickup_DropAirport</t>
+  </si>
+  <si>
+    <t>Car_WithGuestUser_DOMESTIC_Location_DifferentPickup_DropAirport</t>
+  </si>
+  <si>
+    <t>Car_WithGuestUser_DOMESTIC_Location_SamePickupAndDrop_InACity</t>
+  </si>
+  <si>
+    <t>Car_WithGuestUser_DOMESTIC_Location_DifferentPickupAndDrop_InACity</t>
   </si>
 </sst>
 </file>
@@ -200,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -268,26 +299,6 @@
       <top style="thin">
         <color theme="4"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -341,19 +352,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -373,19 +371,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -394,10 +383,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -410,10 +399,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -423,32 +412,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,6 +503,1210 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -560,262 +1762,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1421,6 +2367,70 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color theme="4"/>
@@ -2228,6 +3238,70 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2345,40 +3419,6 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -2515,447 +3555,7 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+      <border outline="0">
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -2965,68 +3565,7 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -3069,245 +3608,13 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3321,43 +3628,7 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -3385,7 +3656,13 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3400,246 +3677,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -3677,156 +3714,156 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="127" dataDxfId="125" headerRowBorderDxfId="126" tableBorderDxfId="124" totalsRowBorderDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="127" dataDxfId="23" headerRowBorderDxfId="126" tableBorderDxfId="125" totalsRowBorderDxfId="124">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="122"/>
+    <tableColumn id="1" name="Description" dataDxfId="4"/>
     <tableColumn id="16" name="ExecutionPipeline" dataDxfId="0"/>
-    <tableColumn id="2" name="PickUpType-Location" dataDxfId="121"/>
-    <tableColumn id="19" name="OriginLocation" dataDxfId="120"/>
-    <tableColumn id="3" name="DropOffType-Location" dataDxfId="119"/>
-    <tableColumn id="20" name="DestinationLocation" dataDxfId="118"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="117"/>
-    <tableColumn id="5" name="RentalAgency" dataDxfId="116"/>
-    <tableColumn id="18" name="CarType" dataDxfId="115"/>
-    <tableColumn id="6" name="AirConditioning" dataDxfId="114"/>
-    <tableColumn id="7" name="Transmission" dataDxfId="113"/>
-    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="112"/>
-    <tableColumn id="9" name="CorpDiscCode" dataDxfId="111"/>
-    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="110"/>
-    <tableColumn id="12" name="UserType" dataDxfId="109"/>
-    <tableColumn id="11" name="PostFilters" dataDxfId="12"/>
-    <tableColumn id="13" name="PostFiltersValues" dataDxfId="11"/>
+    <tableColumn id="2" name="PickUpType-Location" dataDxfId="38"/>
+    <tableColumn id="19" name="OriginLocation" dataDxfId="37"/>
+    <tableColumn id="3" name="DropOffType-Location" dataDxfId="36"/>
+    <tableColumn id="20" name="DestinationLocation" dataDxfId="35"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="34"/>
+    <tableColumn id="5" name="RentalAgency" dataDxfId="33"/>
+    <tableColumn id="18" name="CarType" dataDxfId="32"/>
+    <tableColumn id="6" name="AirConditioning" dataDxfId="31"/>
+    <tableColumn id="7" name="Transmission" dataDxfId="30"/>
+    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="29"/>
+    <tableColumn id="9" name="CorpDiscCode" dataDxfId="28"/>
+    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="27"/>
+    <tableColumn id="12" name="UserType" dataDxfId="26"/>
+    <tableColumn id="11" name="PostFilters" dataDxfId="25"/>
+    <tableColumn id="13" name="PostFiltersValues" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="108" dataDxfId="106" headerRowBorderDxfId="107" tableBorderDxfId="105" totalsRowBorderDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="123" dataDxfId="7" headerRowBorderDxfId="122" tableBorderDxfId="121" totalsRowBorderDxfId="120">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="103"/>
-    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="102"/>
-    <tableColumn id="2" name="PickUpType-Location" dataDxfId="101"/>
-    <tableColumn id="19" name="OriginLocation" dataDxfId="100"/>
-    <tableColumn id="3" name="DropOffType-Location" dataDxfId="99"/>
-    <tableColumn id="20" name="DestinationLocation" dataDxfId="98"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="97"/>
-    <tableColumn id="5" name="RentalAgency" dataDxfId="96"/>
-    <tableColumn id="18" name="CarType" dataDxfId="95"/>
-    <tableColumn id="6" name="AirConditioning" dataDxfId="94"/>
-    <tableColumn id="7" name="Transmission" dataDxfId="93"/>
-    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="92"/>
-    <tableColumn id="9" name="CorpDiscCode" dataDxfId="91"/>
-    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="90"/>
-    <tableColumn id="12" name="UserType" dataDxfId="89"/>
-    <tableColumn id="11" name="PostFilters" dataDxfId="10"/>
-    <tableColumn id="13" name="PostFiltersValues" dataDxfId="9"/>
+    <tableColumn id="1" name="Description" dataDxfId="5"/>
+    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="1"/>
+    <tableColumn id="2" name="PickUpType-Location" dataDxfId="22"/>
+    <tableColumn id="19" name="OriginLocation" dataDxfId="21"/>
+    <tableColumn id="3" name="DropOffType-Location" dataDxfId="20"/>
+    <tableColumn id="20" name="DestinationLocation" dataDxfId="19"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="18"/>
+    <tableColumn id="5" name="RentalAgency" dataDxfId="17"/>
+    <tableColumn id="18" name="CarType" dataDxfId="16"/>
+    <tableColumn id="6" name="AirConditioning" dataDxfId="15"/>
+    <tableColumn id="7" name="Transmission" dataDxfId="14"/>
+    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="13"/>
+    <tableColumn id="9" name="CorpDiscCode" dataDxfId="12"/>
+    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="11"/>
+    <tableColumn id="12" name="UserType" dataDxfId="10"/>
+    <tableColumn id="11" name="PostFilters" dataDxfId="9"/>
+    <tableColumn id="13" name="PostFiltersValues" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="88" dataDxfId="86" headerRowBorderDxfId="87" tableBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="119" dataDxfId="39" headerRowBorderDxfId="118" tableBorderDxfId="117">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="84"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="83"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="82"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="81"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="80"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="79"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="78"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="77"/>
-    <tableColumn id="9" name="CarType" dataDxfId="76"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="75"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="74"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="73"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="72"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="71"/>
-    <tableColumn id="15" name="UserType" dataDxfId="70"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="8"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="7"/>
+    <tableColumn id="1" name="Description" dataDxfId="6"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="2"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="54"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="53"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="52"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="51"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="50"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="49"/>
+    <tableColumn id="9" name="CarType" dataDxfId="48"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="47"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="46"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="45"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="44"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="43"/>
+    <tableColumn id="15" name="UserType" dataDxfId="42"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="41"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="116" dataDxfId="114" headerRowBorderDxfId="115" tableBorderDxfId="113">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="65"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="64"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="63"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="62"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="61"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="60"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="59"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="58"/>
-    <tableColumn id="9" name="CarType" dataDxfId="57"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="56"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="55"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="54"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="53"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="52"/>
-    <tableColumn id="15" name="UserType" dataDxfId="51"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="6"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="5"/>
+    <tableColumn id="1" name="Description" dataDxfId="112"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="3"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="111"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="110"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="109"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="108"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="107"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="106"/>
+    <tableColumn id="9" name="CarType" dataDxfId="105"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="104"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="103"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="102"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="101"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="100"/>
+    <tableColumn id="15" name="UserType" dataDxfId="99"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="98"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="96" dataDxfId="94" headerRowBorderDxfId="95" tableBorderDxfId="93">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="46"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="45"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="44"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="43"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="42"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="41"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="40"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="39"/>
-    <tableColumn id="9" name="CarType" dataDxfId="38"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="37"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="36"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="35"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="34"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="33"/>
-    <tableColumn id="15" name="UserType" dataDxfId="32"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="4"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="3"/>
+    <tableColumn id="1" name="Description" dataDxfId="92"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="91"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="90"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="89"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="88"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="87"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="86"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="85"/>
+    <tableColumn id="9" name="CarType" dataDxfId="84"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="83"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="82"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="81"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="80"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="79"/>
+    <tableColumn id="15" name="UserType" dataDxfId="78"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="77"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="27"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="26"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="25"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="24"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="23"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="22"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="21"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="20"/>
-    <tableColumn id="9" name="CarType" dataDxfId="19"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="18"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="17"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="16"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="15"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="14"/>
-    <tableColumn id="15" name="UserType" dataDxfId="13"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="2"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="1"/>
+    <tableColumn id="1" name="Description" dataDxfId="71"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="70"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="69"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="68"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="67"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="66"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="65"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="64"/>
+    <tableColumn id="9" name="CarType" dataDxfId="63"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="62"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="61"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="60"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="59"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="58"/>
+    <tableColumn id="15" name="UserType" dataDxfId="57"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="56"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4119,17 +4156,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="B9" sqref="B9"/>
+      <selection pane="topRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.5703125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="77.5703125" style="34" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.140625" customWidth="1"/>
@@ -4145,7 +4182,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4160,7 +4197,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -4191,18 +4228,18 @@
         <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>25</v>
+      <c r="A2" s="35" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -4211,7 +4248,7 @@
       <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
@@ -4219,24 +4256,45 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
       <c r="O2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="29" t="s">
-        <v>37</v>
-      </c>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+    </row>
+    <row r="3" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4249,25 +4307,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="1" max="1" width="72.42578125" style="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.140625" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -4282,7 +4343,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -4313,48 +4374,73 @@
         <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>26</v>
+      <c r="A2" s="35" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="29" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+    </row>
+    <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4366,15 +4452,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="72.42578125" style="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
@@ -4392,94 +4478,181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>35</v>
+      <c r="P1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>28</v>
+    <row r="2" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="14" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="32" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+    </row>
+    <row r="3" spans="1:17" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+    </row>
+    <row r="4" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+    </row>
+    <row r="5" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4493,8 +4666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4517,73 +4690,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>35</v>
+      <c r="P1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>29</v>
+      <c r="A2" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" s="16"/>
       <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
@@ -4603,8 +4776,12 @@
       <c r="O2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
+      <c r="P2" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4618,7 +4795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4642,96 +4819,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>35</v>
+      <c r="P1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>31</v>
+      <c r="A2" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="14" t="s">
+      <c r="E2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
+      <c r="P2" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4745,8 +4926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4769,96 +4950,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="M1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q1" s="37" t="s">
-        <v>35</v>
+      <c r="P1" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>32</v>
+      <c r="A2" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4866,4 +5047,39 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Car related bug fixes
updated input data, fix for reading corporate discount code
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/CarScenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="881"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="881" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Car_Airport_To_Airport" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -270,9 +270,6 @@
     <t>Car_WithGuestUser_DOMESTIC_Location_SamePickupAndDrop_InACity_WithCorporateDiscount</t>
   </si>
   <si>
-    <t>CarType|RentalAgency|matrix</t>
-  </si>
-  <si>
     <t>Car_WithLoginMember_DOMESTIC_Location_PickUp_OnAirport_Drop_InACity_SetFilters</t>
   </si>
   <si>
@@ -294,19 +291,16 @@
     <t>0|5</t>
   </si>
   <si>
-    <t>Avis/Hertz</t>
-  </si>
-  <si>
-    <t>Economy/Compact</t>
-  </si>
-  <si>
-    <t>CarType|RentalAgency|Matrix</t>
-  </si>
-  <si>
     <t>Matrix</t>
   </si>
   <si>
     <t>Search|setfilters|AddToCart</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Compact</t>
   </si>
 </sst>
 </file>
@@ -607,203 +601,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -2788,6 +2585,108 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
         <vertical/>
         <horizontal/>
@@ -3198,6 +3097,44 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF000000"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3668,6 +3605,23 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -3763,6 +3717,46 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3866,152 +3860,152 @@
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="121"/>
-    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="0"/>
-    <tableColumn id="2" name="PickUpType-Location" dataDxfId="120"/>
-    <tableColumn id="19" name="OriginLocation" dataDxfId="119"/>
-    <tableColumn id="3" name="DropOffType-Location" dataDxfId="118"/>
-    <tableColumn id="20" name="DestinationLocation" dataDxfId="117"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="116"/>
-    <tableColumn id="5" name="RentalAgency" dataDxfId="115"/>
-    <tableColumn id="18" name="CarType" dataDxfId="6"/>
-    <tableColumn id="6" name="AirConditioning" dataDxfId="114"/>
-    <tableColumn id="7" name="Transmission" dataDxfId="113"/>
-    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="112"/>
-    <tableColumn id="9" name="CorpDiscCode" dataDxfId="111"/>
-    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="110"/>
-    <tableColumn id="12" name="UserType" dataDxfId="109"/>
-    <tableColumn id="11" name="PostFilters" dataDxfId="108"/>
-    <tableColumn id="13" name="PostFiltersValues" dataDxfId="107"/>
+    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="120"/>
+    <tableColumn id="2" name="PickUpType-Location" dataDxfId="119"/>
+    <tableColumn id="19" name="OriginLocation" dataDxfId="118"/>
+    <tableColumn id="3" name="DropOffType-Location" dataDxfId="117"/>
+    <tableColumn id="20" name="DestinationLocation" dataDxfId="116"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="115"/>
+    <tableColumn id="5" name="RentalAgency" dataDxfId="114"/>
+    <tableColumn id="18" name="CarType" dataDxfId="113"/>
+    <tableColumn id="6" name="AirConditioning" dataDxfId="112"/>
+    <tableColumn id="7" name="Transmission" dataDxfId="111"/>
+    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="110"/>
+    <tableColumn id="9" name="CorpDiscCode" dataDxfId="109"/>
+    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="108"/>
+    <tableColumn id="12" name="UserType" dataDxfId="107"/>
+    <tableColumn id="11" name="PostFilters" dataDxfId="106"/>
+    <tableColumn id="13" name="PostFiltersValues" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="106" dataDxfId="104" headerRowBorderDxfId="105" tableBorderDxfId="103" totalsRowBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101" totalsRowBorderDxfId="100">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="101"/>
-    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="100"/>
-    <tableColumn id="2" name="PickUpType-Location" dataDxfId="99"/>
-    <tableColumn id="19" name="OriginLocation" dataDxfId="98"/>
-    <tableColumn id="3" name="DropOffType-Location" dataDxfId="97"/>
-    <tableColumn id="20" name="DestinationLocation" dataDxfId="96"/>
-    <tableColumn id="4" name="TravelDates" dataDxfId="95"/>
-    <tableColumn id="5" name="RentalAgency" dataDxfId="94"/>
-    <tableColumn id="18" name="CarType" dataDxfId="93"/>
-    <tableColumn id="6" name="AirConditioning" dataDxfId="92"/>
-    <tableColumn id="7" name="Transmission" dataDxfId="91"/>
-    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="90"/>
-    <tableColumn id="9" name="CorpDiscCode" dataDxfId="89"/>
-    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="88"/>
-    <tableColumn id="12" name="UserType" dataDxfId="87"/>
-    <tableColumn id="11" name="PostFilters" dataDxfId="5"/>
-    <tableColumn id="13" name="PostFiltersValues" dataDxfId="4"/>
+    <tableColumn id="1" name="Description" dataDxfId="99"/>
+    <tableColumn id="16" name="ExecutionPipeline" dataDxfId="98"/>
+    <tableColumn id="2" name="PickUpType-Location" dataDxfId="97"/>
+    <tableColumn id="19" name="OriginLocation" dataDxfId="96"/>
+    <tableColumn id="3" name="DropOffType-Location" dataDxfId="95"/>
+    <tableColumn id="20" name="DestinationLocation" dataDxfId="94"/>
+    <tableColumn id="4" name="TravelDates" dataDxfId="93"/>
+    <tableColumn id="5" name="RentalAgency" dataDxfId="92"/>
+    <tableColumn id="18" name="CarType" dataDxfId="91"/>
+    <tableColumn id="6" name="AirConditioning" dataDxfId="90"/>
+    <tableColumn id="7" name="Transmission" dataDxfId="89"/>
+    <tableColumn id="8" name="CorpDiscRentalAgency" dataDxfId="88"/>
+    <tableColumn id="9" name="CorpDiscCode" dataDxfId="87"/>
+    <tableColumn id="10" name="CorpDiscPromotionalCode" dataDxfId="86"/>
+    <tableColumn id="12" name="UserType" dataDxfId="85"/>
+    <tableColumn id="11" name="PostFilters" dataDxfId="84"/>
+    <tableColumn id="13" name="PostFiltersValues" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="82" dataDxfId="80" headerRowBorderDxfId="81" tableBorderDxfId="79">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="82"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="81"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="80"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="79"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="78"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="77"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="76"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="75"/>
-    <tableColumn id="9" name="CarType" dataDxfId="74"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="73"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="72"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="3"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="2"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="1"/>
-    <tableColumn id="15" name="UserType" dataDxfId="71"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="70"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="69"/>
+    <tableColumn id="1" name="Description" dataDxfId="78"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="77"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="76"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="75"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="74"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="73"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="72"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="71"/>
+    <tableColumn id="9" name="CarType" dataDxfId="70"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="69"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="68"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="67"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="66"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="65"/>
+    <tableColumn id="15" name="UserType" dataDxfId="64"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="63"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="65"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="64"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="63"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="62"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="61"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="60"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="59"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="58"/>
-    <tableColumn id="9" name="CarType" dataDxfId="57"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="56"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="55"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="54"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="53"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="52"/>
-    <tableColumn id="15" name="UserType" dataDxfId="51"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="50"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="49"/>
+    <tableColumn id="1" name="Description" dataDxfId="58"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="57"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="56"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="55"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="54"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="53"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="52"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="51"/>
+    <tableColumn id="9" name="CarType" dataDxfId="50"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="49"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="48"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="47"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="46"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="45"/>
+    <tableColumn id="15" name="UserType" dataDxfId="44"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="43"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="44"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="43"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="42"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="41"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="40"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="39"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="38"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="37"/>
-    <tableColumn id="9" name="CarType" dataDxfId="36"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="35"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="34"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="33"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="32"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="31"/>
-    <tableColumn id="15" name="UserType" dataDxfId="30"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="29"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="28"/>
+    <tableColumn id="1" name="Description" dataDxfId="37"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="36"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="35"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="34"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="33"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="32"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="31"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="30"/>
+    <tableColumn id="9" name="CarType" dataDxfId="29"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="28"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="27"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="26"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="25"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="24"/>
+    <tableColumn id="15" name="UserType" dataDxfId="23"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="22"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="23"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="22"/>
-    <tableColumn id="3" name="PickUpType-Location" dataDxfId="21"/>
-    <tableColumn id="4" name="OriginLocation" dataDxfId="20"/>
-    <tableColumn id="5" name="DropOffType-Location" dataDxfId="19"/>
-    <tableColumn id="6" name="DestinationLocation" dataDxfId="18"/>
-    <tableColumn id="7" name="TravelDates" dataDxfId="17"/>
-    <tableColumn id="8" name="RentalAgency" dataDxfId="16"/>
-    <tableColumn id="9" name="CarType" dataDxfId="15"/>
-    <tableColumn id="10" name="AirConditioning" dataDxfId="14"/>
-    <tableColumn id="11" name="Transmission" dataDxfId="13"/>
-    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="12"/>
-    <tableColumn id="13" name="CorpDiscCode" dataDxfId="11"/>
-    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="10"/>
-    <tableColumn id="15" name="UserType" dataDxfId="9"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="8"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="7"/>
+    <tableColumn id="1" name="Description" dataDxfId="16"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="15"/>
+    <tableColumn id="3" name="PickUpType-Location" dataDxfId="14"/>
+    <tableColumn id="4" name="OriginLocation" dataDxfId="13"/>
+    <tableColumn id="5" name="DropOffType-Location" dataDxfId="12"/>
+    <tableColumn id="6" name="DestinationLocation" dataDxfId="11"/>
+    <tableColumn id="7" name="TravelDates" dataDxfId="10"/>
+    <tableColumn id="8" name="RentalAgency" dataDxfId="9"/>
+    <tableColumn id="9" name="CarType" dataDxfId="8"/>
+    <tableColumn id="10" name="AirConditioning" dataDxfId="7"/>
+    <tableColumn id="11" name="Transmission" dataDxfId="6"/>
+    <tableColumn id="12" name="CorpDiscRentalAgency" dataDxfId="5"/>
+    <tableColumn id="13" name="CorpDiscCode" dataDxfId="4"/>
+    <tableColumn id="14" name="CorpDiscPromotionalCode" dataDxfId="3"/>
+    <tableColumn id="15" name="UserType" dataDxfId="2"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="1"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4306,10 +4300,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4"/>
+      <selection pane="topRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4460,7 +4454,7 @@
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -4623,7 +4617,7 @@
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -4658,7 +4652,7 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -4722,7 +4716,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4796,10 +4790,10 @@
     </row>
     <row r="2" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" s="23" t="s">
         <v>22</v>
@@ -4831,10 +4825,10 @@
     </row>
     <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>22</v>
@@ -4866,10 +4860,10 @@
     </row>
     <row r="4" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>22</v>
@@ -4901,10 +4895,10 @@
     </row>
     <row r="5" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>22</v>
@@ -4928,15 +4922,15 @@
         <v>35</v>
       </c>
       <c r="P5" s="33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C6" s="23" t="s">
         <v>22</v>
@@ -4960,7 +4954,7 @@
         <v>35</v>
       </c>
       <c r="P6" s="36" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="36" t="s">
         <v>65</v>
@@ -4979,8 +4973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5133,7 +5127,7 @@
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -5167,7 +5161,7 @@
         <v>6</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -5296,7 +5290,7 @@
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -5330,7 +5324,7 @@
         <v>6</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -5393,8 +5387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5471,7 +5465,7 @@
     </row>
     <row r="2" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>61</v>
@@ -5498,7 +5492,7 @@
         <v>35</v>
       </c>
       <c r="P2" s="36" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="Q2" s="36" t="s">
         <v>65</v>
@@ -5506,7 +5500,7 @@
     </row>
     <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>61</v>
@@ -5541,7 +5535,7 @@
     </row>
     <row r="4" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>61</v>
@@ -5576,7 +5570,7 @@
     </row>
     <row r="5" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>61</v>
@@ -5611,7 +5605,7 @@
     </row>
     <row r="6" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>61</v>
@@ -5814,7 +5808,7 @@
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -5987,7 +5981,7 @@
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -6248,7 +6242,7 @@
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -6421,7 +6415,7 @@
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>

</xml_diff>